<commit_message>
tests: validate simple data file loading
</commit_message>
<xml_diff>
--- a/tests/data/test_loader/res_partner.xlsx
+++ b/tests/data/test_loader/res_partner.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="res.partner" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Import FAQ" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -21,54 +21,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
-  <si>
-    <t xml:space="preserve">External ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Company Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">res_partner_1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state_id/id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__import__.res_partner_1</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Grocery Outlet</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">San Francisco</t>
   </si>
   <si>
-    <t xml:space="preserve">CA</t>
+    <t xml:space="preserve">base.state_us_5</t>
   </si>
   <si>
     <t xml:space="preserve">US</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">groceryoutlet.com</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_2</t>
+    <t xml:space="preserve">__import__.res_partner_2</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Bob</t>
@@ -104,13 +104,10 @@
     <t xml:space="preserve">Individual</t>
   </si>
   <si>
-    <t xml:space="preserve">Grocery Outlet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contact</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_3</t>
+    <t xml:space="preserve">__import__.res_partner_3</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Bill</t>
@@ -122,7 +119,7 @@
     <t xml:space="preserve">645 21st Street</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_4</t>
+    <t xml:space="preserve">__import__.res_partner_4</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Warehouse</t>
@@ -134,7 +131,7 @@
     <t xml:space="preserve">bill@grocery-outlet.com</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_5</t>
+    <t xml:space="preserve">__import__.res_partner_5</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Accounting dep.</t>
@@ -146,7 +143,7 @@
     <t xml:space="preserve">#404</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_6</t>
+    <t xml:space="preserve">__import__.res_partner_6</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX ASUSTeK</t>
@@ -158,13 +155,13 @@
     <t xml:space="preserve">New York</t>
   </si>
   <si>
-    <t xml:space="preserve">NY</t>
+    <t xml:space="preserve">base.state_us_27</t>
   </si>
   <si>
     <t xml:space="preserve">asustek.com</t>
   </si>
   <si>
-    <t xml:space="preserve">res_partner_7</t>
+    <t xml:space="preserve">__import__.res_partner_7</t>
   </si>
   <si>
     <t xml:space="preserve">XLSX Camptocamp</t>
@@ -547,13 +544,14 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.13"/>
@@ -656,10 +654,10 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -676,22 +674,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2" t="s">
@@ -715,22 +713,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
@@ -751,30 +749,30 @@
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>20</v>
@@ -797,10 +795,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
@@ -808,14 +806,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>11201</v>
@@ -824,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>654978123</v>
@@ -834,10 +832,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
@@ -845,18 +843,18 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="2" t="n">
         <v>73377</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -897,32 +895,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,17 +928,17 @@
     </row>
     <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,27 +946,27 @@
     </row>
     <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,22 +974,22 @@
     </row>
     <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,17 +997,17 @@
     </row>
     <row r="23" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,22 +1015,22 @@
     </row>
     <row r="27" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,12 +1038,12 @@
     </row>
     <row r="32" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
[FIX] adapt data to 8.0 compatibility
</commit_message>
<xml_diff>
--- a/tests/data/test_loader/res_partner.xlsx
+++ b/tests/data/test_loader/res_partner.xlsx
@@ -29,7 +29,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">company_type</t>
+    <t xml:space="preserve">is_company</t>
   </si>
   <si>
     <t xml:space="preserve">parent_id</t>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">XLSX Grocery Outlet</t>
   </si>
   <si>
-    <t xml:space="preserve">Company</t>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">51 Federal Street</t>
@@ -101,10 +101,10 @@
     <t xml:space="preserve">XLSX Bob</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact</t>
   </si>
   <si>
     <t xml:space="preserve">__import__.res_partner_3</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">XLSX Bill</t>
   </si>
   <si>
-    <t xml:space="preserve">Other address</t>
+    <t xml:space="preserve">other</t>
   </si>
   <si>
     <t xml:space="preserve">645 21st Street</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">XLSX Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Shipping address</t>
+    <t xml:space="preserve">delivery</t>
   </si>
   <si>
     <t xml:space="preserve">bill@grocery-outlet.com</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">XLSX Accounting dep.</t>
   </si>
   <si>
-    <t xml:space="preserve">Invoice address</t>
+    <t xml:space="preserve">invoice</t>
   </si>
   <si>
     <t xml:space="preserve">#404</t>
@@ -544,7 +544,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>